<commit_message>
Remove date_with_text and new function
Loose code was converted to rename_sample_id_column function and everything related to the date_with_text function was deleted.
</commit_message>
<xml_diff>
--- a/inst/extdata/Metadata_example.xlsx
+++ b/inst/extdata/Metadata_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slsiekman\Documents\glycodash\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1FE180A-3AE9-4223-A736-3DEC064EAB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB81DD7F-EAC1-40B9-A598-28D7BBE2819E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5175A5A9-D43F-4EE2-8721-AD3F14EF0F6C}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="12735" xr2:uid="{5175A5A9-D43F-4EE2-8721-AD3F14EF0F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>sample_id</t>
-  </si>
-  <si>
     <t>PBS</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
   </si>
 </sst>
 </file>
@@ -422,9 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{814D656C-F006-4CC1-9354-42AFFD3CAC7B}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -434,21 +432,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -456,10 +454,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -467,10 +465,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -478,10 +476,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>

</xml_diff>